<commit_message>
EEPROM setup over serial PoC
</commit_message>
<xml_diff>
--- a/PCB/fanControl/RFQ/fanControl_stock.xlsx
+++ b/PCB/fanControl/RFQ/fanControl_stock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakad\source\repos\fanControl\PCB\fanControl\RFQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17BCDDC-BC14-4B9D-92F9-117299490F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0A6D26-1881-4D81-AEF9-707F58B248D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fanControl_RFQ1!$A$1:$K$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">fanControl_RFQ2_1!$A$1:$N$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stock!$A$1:$K$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stock!$A$1:$K$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="305">
   <si>
     <t>Reference</t>
   </si>
@@ -933,6 +933,27 @@
   </si>
   <si>
     <t>RC0805FR-070RL</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>BC547</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_THT:TO-92_Inline_Wide</t>
+  </si>
+  <si>
+    <t>BC547B</t>
+  </si>
+  <si>
+    <t>CDIL</t>
+  </si>
+  <si>
+    <t>https://arwill.hu/termekek/felvezetok/tranzisztorok/bc/bc547b-tranzisztor-160303/</t>
+  </si>
+  <si>
+    <t>https://arwill.hu/forras/termek/felvezetok/tranzisztorok/bc/bc547b-tranzisztor-160303.pdf</t>
   </si>
 </sst>
 </file>
@@ -1808,11 +1829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7463E6FB-AFB1-4949-90AE-CE9BA08FB519}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1989,7 @@
         <v>34</v>
       </c>
       <c r="K5">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2055,7 +2076,7 @@
         <v>45</v>
       </c>
       <c r="K8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2366,7 +2387,7 @@
         <v>106</v>
       </c>
       <c r="K18">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2389,7 +2410,7 @@
         <v>109</v>
       </c>
       <c r="K19">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3066,370 +3087,325 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>240</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
+        <v>241</v>
+      </c>
+      <c r="F41" t="s">
+        <v>242</v>
+      </c>
+      <c r="G41" t="s">
+        <v>243</v>
+      </c>
+      <c r="H41" t="s">
+        <v>64</v>
       </c>
       <c r="I41" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="K41">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>245</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>246</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>247</v>
+      </c>
+      <c r="E42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F42" t="s">
+        <v>249</v>
+      </c>
+      <c r="G42" t="s">
+        <v>250</v>
+      </c>
+      <c r="H42" t="s">
+        <v>251</v>
       </c>
       <c r="I42" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="K42">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>256</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="F43" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="G43" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="H43" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="I43" t="s">
         <v>17</v>
       </c>
       <c r="K43">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="D44" t="s">
-        <v>247</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="F44" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="G44" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="H44" t="s">
-        <v>251</v>
+        <v>64</v>
       </c>
       <c r="I44" t="s">
         <v>17</v>
       </c>
       <c r="K44">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>287</v>
       </c>
       <c r="D45" t="s">
-        <v>252</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
-        <v>253</v>
-      </c>
-      <c r="G45">
-        <v>694106301002</v>
+        <v>288</v>
+      </c>
+      <c r="F45" t="s">
+        <v>289</v>
+      </c>
+      <c r="G45" t="s">
+        <v>290</v>
       </c>
       <c r="H45" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="I45" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="K45">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>267</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>138</v>
+      </c>
+      <c r="E46" t="s">
+        <v>268</v>
+      </c>
+      <c r="F46" t="s">
+        <v>269</v>
+      </c>
+      <c r="G46" t="s">
+        <v>270</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
       </c>
       <c r="I46" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="K46">
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>257</v>
+        <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="E47" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="F47" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G47" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="H47" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="I47" t="s">
         <v>17</v>
       </c>
       <c r="K47">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>261</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="F48" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="G48" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="H48" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="I48" t="s">
         <v>17</v>
       </c>
       <c r="K48">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>129</v>
+      <c r="A49" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>287</v>
-      </c>
-      <c r="D49" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" t="s">
-        <v>288</v>
+        <v>295</v>
+      </c>
+      <c r="D49" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="F49" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="G49" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="H49" t="s">
-        <v>291</v>
+        <v>16</v>
       </c>
       <c r="I49" t="s">
         <v>17</v>
       </c>
       <c r="K49">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>267</v>
+        <v>299</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="E50" t="s">
-        <v>268</v>
-      </c>
-      <c r="F50" t="s">
-        <v>269</v>
+        <v>304</v>
       </c>
       <c r="G50" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="H50" t="s">
-        <v>16</v>
+        <v>302</v>
       </c>
       <c r="I50" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="K50">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>271</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>153</v>
-      </c>
-      <c r="D51" t="s">
-        <v>138</v>
-      </c>
-      <c r="E51" t="s">
-        <v>272</v>
-      </c>
-      <c r="F51" t="s">
-        <v>273</v>
-      </c>
-      <c r="G51" t="s">
-        <v>274</v>
-      </c>
-      <c r="H51" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>277</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" t="s">
-        <v>138</v>
-      </c>
-      <c r="E52" t="s">
-        <v>278</v>
-      </c>
-      <c r="F52" t="s">
-        <v>279</v>
-      </c>
-      <c r="G52" t="s">
-        <v>280</v>
-      </c>
-      <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>17</v>
-      </c>
-      <c r="K52">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>295</v>
-      </c>
-      <c r="D53" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F53" t="s">
-        <v>296</v>
-      </c>
-      <c r="G53" t="s">
-        <v>297</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" t="s">
-        <v>17</v>
-      </c>
-      <c r="K53">
-        <v>100</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K53" xr:uid="{7463E6FB-AFB1-4949-90AE-CE9BA08FB519}"/>
+  <autoFilter ref="A1:K50" xr:uid="{7463E6FB-AFB1-4949-90AE-CE9BA08FB519}"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{E9F6D936-1813-47E7-B657-345F6EC176C0}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{62210B75-87B6-4ABF-8122-84E9278A0507}"/>
@@ -3469,6 +3445,7 @@
     <hyperlink ref="J8" r:id="rId36" xr:uid="{0B59B73A-0FD6-4FA1-89BE-7F21F1BFA19A}"/>
     <hyperlink ref="J18" r:id="rId37" xr:uid="{DE2B6A7E-3F2A-4310-B553-88E952BC70E2}"/>
     <hyperlink ref="J19" r:id="rId38" xr:uid="{6CFA8BD4-57C6-4535-BB15-1425A8D1066A}"/>
+    <hyperlink ref="J50" r:id="rId39" xr:uid="{08C7C7F2-BF9E-435B-952F-B86EFAEC292B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>